<commit_message>
added manual supp data in scripts for CM, D, M
</commit_message>
<xml_diff>
--- a/in/extraction1/corrections/supp_CM.xlsx
+++ b/in/extraction1/corrections/supp_CM.xlsx
@@ -99,9 +99,6 @@
     <t>Sarkozy</t>
   </si>
   <si>
-    <t>Population de la commune</t>
-  </si>
-  <si>
     <t>Neuilly-sur-Seine</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t>Maire</t>
+  </si>
+  <si>
+    <t>Population commune</t>
   </si>
 </sst>
 </file>
@@ -959,9 +959,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection sqref="A1:U2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -969,7 +967,7 @@
     <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
@@ -996,13 +994,13 @@
         <v>18</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="10" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="F1" s="10" t="s">
         <v>7</v>
@@ -1061,13 +1059,13 @@
         <v>23</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>24</v>
@@ -1097,7 +1095,7 @@
         <v>5</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P2" s="6">
         <v>30435</v>

</xml_diff>

<commit_message>
minor fixes in the integration of manual data
</commit_message>
<xml_diff>
--- a/in/extraction1/corrections/supp_CM.xlsx
+++ b/in/extraction1/corrections/supp_CM.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22730"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Vincent\eclipse\workspaces\Extraction\Datapol\in\extraction1\corrections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vincent\eclipse\workspaces\Extraction\Datapol\in\extraction1\corrections\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B557CFE-ADE6-4172-B69E-01EED64DB2B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Liste" sheetId="4" r:id="rId1"/>
@@ -123,7 +124,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -638,48 +639,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -956,37 +957,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="18.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="18.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.54296875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.1796875" style="3" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="6.81640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="11" t="s">
         <v>17</v>
       </c>
@@ -1051,7 +1052,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>92</v>
       </c>
@@ -1116,7 +1117,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4"/>
       <c r="C3" s="4"/>
       <c r="E3" s="4"/>
@@ -1125,7 +1126,7 @@
       <c r="N3" s="8"/>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="4"/>
       <c r="C4" s="4"/>
       <c r="E4" s="4"/>
@@ -1134,17 +1135,11 @@
       <c r="N4" s="8"/>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="N5" s="8"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="9"/>
-    </row>
-    <row r="6" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="O5" s="4"/>
+      <c r="S5" s="9"/>
+    </row>
+    <row r="6" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="4"/>
       <c r="C6" s="4"/>
       <c r="E6" s="4"/>
@@ -1154,7 +1149,7 @@
       <c r="O6" s="9"/>
       <c r="P6" s="9"/>
     </row>
-    <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="4"/>
       <c r="C7" s="4"/>
       <c r="E7" s="4"/>
@@ -1162,7 +1157,7 @@
       <c r="K7" s="6"/>
       <c r="N7" s="7"/>
     </row>
-    <row r="8" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4"/>
       <c r="C8" s="4"/>
       <c r="E8" s="4"/>
@@ -1170,7 +1165,7 @@
       <c r="K8" s="6"/>
       <c r="N8" s="7"/>
     </row>
-    <row r="9" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4"/>
       <c r="C9" s="4"/>
       <c r="E9" s="4"/>
@@ -1180,7 +1175,7 @@
       <c r="O9" s="9"/>
       <c r="P9" s="9"/>
     </row>
-    <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A10" s="4"/>
       <c r="C10" s="4"/>
       <c r="E10" s="4"/>
@@ -1188,7 +1183,7 @@
       <c r="K10" s="6"/>
       <c r="N10" s="7"/>
     </row>
-    <row r="11" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="4"/>
       <c r="C11" s="4"/>
       <c r="E11" s="4"/>
@@ -1197,7 +1192,7 @@
       <c r="N11" s="8"/>
       <c r="O11" s="9"/>
     </row>
-    <row r="12" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="C12" s="4"/>
       <c r="E12" s="4"/>
@@ -1207,7 +1202,7 @@
       <c r="O12" s="9"/>
       <c r="P12" s="9"/>
     </row>
-    <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="4"/>
       <c r="C13" s="4"/>
       <c r="E13" s="4"/>
@@ -1216,7 +1211,7 @@
       <c r="N13" s="8"/>
       <c r="O13" s="9"/>
     </row>
-    <row r="14" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4"/>
       <c r="C14" s="4"/>
       <c r="E14" s="4"/>
@@ -1226,7 +1221,7 @@
       <c r="O14" s="9"/>
       <c r="P14" s="9"/>
     </row>
-    <row r="15" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4"/>
       <c r="C15" s="4"/>
       <c r="E15" s="4"/>
@@ -1235,7 +1230,7 @@
       <c r="N15" s="8"/>
       <c r="O15" s="9"/>
     </row>
-    <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4"/>
       <c r="C16" s="4"/>
       <c r="E16" s="4"/>
@@ -1245,7 +1240,7 @@
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
     </row>
-    <row r="17" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4"/>
       <c r="C17" s="4"/>
       <c r="E17" s="4"/>
@@ -1253,7 +1248,7 @@
       <c r="K17" s="6"/>
       <c r="N17" s="7"/>
     </row>
-    <row r="18" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4"/>
       <c r="C18" s="4"/>
       <c r="E18" s="4"/>
@@ -1263,7 +1258,7 @@
       <c r="O18" s="9"/>
       <c r="P18" s="9"/>
     </row>
-    <row r="19" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="4"/>
       <c r="C19" s="4"/>
       <c r="E19" s="4"/>
@@ -1271,7 +1266,7 @@
       <c r="K19" s="6"/>
       <c r="N19" s="7"/>
     </row>
-    <row r="20" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="C20" s="4"/>
       <c r="E20" s="4"/>
@@ -1279,7 +1274,7 @@
       <c r="K20" s="6"/>
       <c r="N20" s="7"/>
     </row>
-    <row r="21" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="C21" s="4"/>
       <c r="E21" s="4"/>
@@ -1289,7 +1284,7 @@
       <c r="O21" s="9"/>
       <c r="P21" s="9"/>
     </row>
-    <row r="22" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="4"/>
       <c r="C22" s="4"/>
       <c r="E22" s="4"/>
@@ -1299,7 +1294,7 @@
       <c r="O22" s="9"/>
       <c r="P22" s="9"/>
     </row>
-    <row r="23" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="4"/>
       <c r="C23" s="4"/>
       <c r="E23" s="4"/>
@@ -1309,7 +1304,7 @@
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
     </row>
-    <row r="24" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="4"/>
       <c r="C24" s="4"/>
       <c r="E24" s="4"/>
@@ -1317,7 +1312,7 @@
       <c r="K24" s="6"/>
       <c r="N24" s="7"/>
     </row>
-    <row r="25" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="4"/>
       <c r="C25" s="4"/>
       <c r="E25" s="4"/>
@@ -1327,7 +1322,7 @@
       <c r="O25" s="9"/>
       <c r="P25" s="9"/>
     </row>
-    <row r="26" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
       <c r="C26" s="4"/>
       <c r="E26" s="4"/>
@@ -1335,7 +1330,7 @@
       <c r="K26" s="6"/>
       <c r="N26" s="7"/>
     </row>
-    <row r="27" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
       <c r="C27" s="4"/>
       <c r="E27" s="4"/>
@@ -1345,7 +1340,7 @@
       <c r="O27" s="9"/>
       <c r="P27" s="9"/>
     </row>
-    <row r="28" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
       <c r="C28" s="4"/>
       <c r="E28" s="4"/>
@@ -1355,7 +1350,7 @@
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
     </row>
-    <row r="29" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>
       <c r="C29" s="4"/>
       <c r="E29" s="4"/>
@@ -1364,7 +1359,7 @@
       <c r="N29" s="8"/>
       <c r="O29" s="9"/>
     </row>
-    <row r="30" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
       <c r="C30" s="4"/>
       <c r="E30" s="4"/>
@@ -1374,7 +1369,7 @@
       <c r="O30" s="9"/>
       <c r="P30" s="9"/>
     </row>
-    <row r="31" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
       <c r="C31" s="4"/>
       <c r="E31" s="4"/>
@@ -1382,7 +1377,7 @@
       <c r="K31" s="6"/>
       <c r="N31" s="7"/>
     </row>
-    <row r="32" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
       <c r="C32" s="4"/>
       <c r="E32" s="4"/>
@@ -1390,7 +1385,7 @@
       <c r="K32" s="6"/>
       <c r="N32" s="7"/>
     </row>
-    <row r="33" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
       <c r="C33" s="4"/>
       <c r="E33" s="4"/>
@@ -1400,7 +1395,7 @@
       <c r="O33" s="9"/>
       <c r="P33" s="9"/>
     </row>
-    <row r="34" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
       <c r="C34" s="4"/>
       <c r="E34" s="4"/>
@@ -1410,7 +1405,7 @@
       <c r="O34" s="9"/>
       <c r="P34" s="9"/>
     </row>
-    <row r="35" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
       <c r="C35" s="4"/>
       <c r="E35" s="4"/>
@@ -1420,7 +1415,7 @@
       <c r="O35" s="9"/>
       <c r="P35" s="9"/>
     </row>
-    <row r="36" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
       <c r="C36" s="4"/>
       <c r="E36" s="4"/>
@@ -1430,7 +1425,7 @@
       <c r="O36" s="9"/>
       <c r="P36" s="9"/>
     </row>
-    <row r="37" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>
       <c r="C37" s="4"/>
       <c r="E37" s="4"/>
@@ -1438,7 +1433,7 @@
       <c r="K37" s="6"/>
       <c r="N37" s="7"/>
     </row>
-    <row r="38" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
       <c r="C38" s="4"/>
       <c r="E38" s="4"/>
@@ -1446,7 +1441,7 @@
       <c r="K38" s="6"/>
       <c r="N38" s="7"/>
     </row>
-    <row r="39" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
       <c r="C39" s="4"/>
       <c r="E39" s="4"/>
@@ -1454,7 +1449,7 @@
       <c r="K39" s="6"/>
       <c r="N39" s="7"/>
     </row>
-    <row r="40" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="4"/>
       <c r="C40" s="4"/>
       <c r="E40" s="4"/>
@@ -1464,7 +1459,7 @@
       <c r="O40" s="9"/>
       <c r="P40" s="9"/>
     </row>
-    <row r="41" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="4"/>
       <c r="C41" s="4"/>
       <c r="E41" s="4"/>
@@ -1474,7 +1469,7 @@
       <c r="O41" s="9"/>
       <c r="P41" s="9"/>
     </row>
-    <row r="42" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="4"/>
       <c r="C42" s="4"/>
       <c r="E42" s="4"/>
@@ -1484,7 +1479,7 @@
       <c r="O42" s="9"/>
       <c r="P42" s="9"/>
     </row>
-    <row r="43" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4"/>
       <c r="C43" s="4"/>
       <c r="E43" s="4"/>
@@ -1493,7 +1488,7 @@
       <c r="N43" s="8"/>
       <c r="O43" s="9"/>
     </row>
-    <row r="44" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="4"/>
       <c r="C44" s="4"/>
       <c r="E44" s="4"/>
@@ -1503,7 +1498,7 @@
       <c r="O44" s="9"/>
       <c r="P44" s="9"/>
     </row>
-    <row r="45" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A45" s="4"/>
       <c r="C45" s="4"/>
       <c r="E45" s="4"/>
@@ -1512,7 +1507,7 @@
       <c r="N45" s="8"/>
       <c r="O45" s="9"/>
     </row>
-    <row r="46" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="4"/>
       <c r="C46" s="4"/>
       <c r="E46" s="4"/>
@@ -1520,7 +1515,7 @@
       <c r="K46" s="6"/>
       <c r="N46" s="7"/>
     </row>
-    <row r="47" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="4"/>
       <c r="C47" s="4"/>
       <c r="E47" s="4"/>
@@ -1528,7 +1523,7 @@
       <c r="K47" s="6"/>
       <c r="N47" s="7"/>
     </row>
-    <row r="48" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A48" s="4"/>
       <c r="C48" s="4"/>
       <c r="E48" s="4"/>
@@ -1536,7 +1531,7 @@
       <c r="K48" s="6"/>
       <c r="N48" s="7"/>
     </row>
-    <row r="49" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="4"/>
       <c r="C49" s="4"/>
       <c r="E49" s="4"/>
@@ -1545,7 +1540,7 @@
       <c r="N49" s="8"/>
       <c r="O49" s="9"/>
     </row>
-    <row r="50" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4"/>
       <c r="C50" s="4"/>
       <c r="E50" s="4"/>
@@ -1553,7 +1548,7 @@
       <c r="K50" s="6"/>
       <c r="N50" s="7"/>
     </row>
-    <row r="51" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="4"/>
       <c r="C51" s="4"/>
       <c r="E51" s="4"/>
@@ -1562,7 +1557,7 @@
       <c r="N51" s="8"/>
       <c r="O51" s="9"/>
     </row>
-    <row r="52" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A52" s="4"/>
       <c r="C52" s="4"/>
       <c r="E52" s="4"/>
@@ -1572,7 +1567,7 @@
       <c r="O52" s="9"/>
       <c r="P52" s="9"/>
     </row>
-    <row r="53" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A53" s="4"/>
       <c r="C53" s="4"/>
       <c r="E53" s="4"/>
@@ -1580,7 +1575,7 @@
       <c r="K53" s="6"/>
       <c r="N53" s="7"/>
     </row>
-    <row r="54" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="4"/>
       <c r="C54" s="4"/>
       <c r="E54" s="4"/>
@@ -1588,7 +1583,7 @@
       <c r="K54" s="6"/>
       <c r="N54" s="7"/>
     </row>
-    <row r="55" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="4"/>
       <c r="C55" s="4"/>
       <c r="E55" s="4"/>
@@ -1598,7 +1593,7 @@
       <c r="O55" s="9"/>
       <c r="P55" s="9"/>
     </row>
-    <row r="56" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4"/>
       <c r="C56" s="4"/>
       <c r="E56" s="4"/>
@@ -1608,7 +1603,7 @@
       <c r="O56" s="9"/>
       <c r="P56" s="9"/>
     </row>
-    <row r="57" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A57" s="4"/>
       <c r="C57" s="4"/>
       <c r="E57" s="4"/>
@@ -1618,7 +1613,7 @@
       <c r="O57" s="9"/>
       <c r="P57" s="9"/>
     </row>
-    <row r="58" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="4"/>
       <c r="C58" s="4"/>
       <c r="E58" s="4"/>
@@ -1628,7 +1623,7 @@
       <c r="O58" s="9"/>
       <c r="P58" s="9"/>
     </row>
-    <row r="59" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A59" s="4"/>
       <c r="C59" s="4"/>
       <c r="E59" s="4"/>
@@ -1638,7 +1633,7 @@
       <c r="O59" s="9"/>
       <c r="P59" s="9"/>
     </row>
-    <row r="60" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A60" s="4"/>
       <c r="C60" s="4"/>
       <c r="E60" s="4"/>
@@ -1648,7 +1643,7 @@
       <c r="O60" s="9"/>
       <c r="P60" s="9"/>
     </row>
-    <row r="61" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A61" s="4"/>
       <c r="C61" s="4"/>
       <c r="E61" s="4"/>
@@ -1658,7 +1653,7 @@
       <c r="O61" s="9"/>
       <c r="P61" s="9"/>
     </row>
-    <row r="62" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A62" s="4"/>
       <c r="C62" s="4"/>
       <c r="E62" s="4"/>
@@ -1668,7 +1663,7 @@
       <c r="O62" s="9"/>
       <c r="P62" s="9"/>
     </row>
-    <row r="63" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A63" s="4"/>
       <c r="C63" s="4"/>
       <c r="E63" s="4"/>
@@ -1676,7 +1671,7 @@
       <c r="K63" s="6"/>
       <c r="N63" s="7"/>
     </row>
-    <row r="64" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A64" s="4"/>
       <c r="C64" s="4"/>
       <c r="E64" s="4"/>
@@ -1684,7 +1679,7 @@
       <c r="K64" s="6"/>
       <c r="N64" s="7"/>
     </row>
-    <row r="65" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A65" s="4"/>
       <c r="C65" s="4"/>
       <c r="E65" s="4"/>
@@ -1692,7 +1687,7 @@
       <c r="K65" s="6"/>
       <c r="N65" s="7"/>
     </row>
-    <row r="66" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A66" s="4"/>
       <c r="C66" s="4"/>
       <c r="E66" s="4"/>
@@ -1700,7 +1695,7 @@
       <c r="K66" s="6"/>
       <c r="N66" s="7"/>
     </row>
-    <row r="67" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A67" s="4"/>
       <c r="C67" s="4"/>
       <c r="E67" s="4"/>
@@ -1710,7 +1705,7 @@
       <c r="O67" s="9"/>
       <c r="P67" s="9"/>
     </row>
-    <row r="68" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A68" s="4"/>
       <c r="C68" s="4"/>
       <c r="E68" s="4"/>
@@ -1720,7 +1715,7 @@
       <c r="O68" s="9"/>
       <c r="P68" s="9"/>
     </row>
-    <row r="69" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A69" s="4"/>
       <c r="C69" s="4"/>
       <c r="E69" s="4"/>
@@ -1728,7 +1723,7 @@
       <c r="K69" s="6"/>
       <c r="N69" s="7"/>
     </row>
-    <row r="70" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A70" s="4"/>
       <c r="C70" s="4"/>
       <c r="E70" s="4"/>
@@ -1738,7 +1733,7 @@
       <c r="O70" s="9"/>
       <c r="P70" s="9"/>
     </row>
-    <row r="71" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A71" s="4"/>
       <c r="C71" s="4"/>
       <c r="E71" s="4"/>
@@ -1748,7 +1743,7 @@
       <c r="O71" s="9"/>
       <c r="P71" s="9"/>
     </row>
-    <row r="72" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A72" s="4"/>
       <c r="C72" s="4"/>
       <c r="E72" s="4"/>
@@ -1756,7 +1751,7 @@
       <c r="K72" s="6"/>
       <c r="N72" s="7"/>
     </row>
-    <row r="73" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A73" s="4"/>
       <c r="C73" s="4"/>
       <c r="E73" s="4"/>
@@ -1765,7 +1760,7 @@
       <c r="N73" s="8"/>
       <c r="O73" s="9"/>
     </row>
-    <row r="74" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A74" s="4"/>
       <c r="C74" s="4"/>
       <c r="E74" s="4"/>
@@ -1774,7 +1769,7 @@
       <c r="N74" s="8"/>
       <c r="O74" s="9"/>
     </row>
-    <row r="75" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A75" s="4"/>
       <c r="C75" s="4"/>
       <c r="E75" s="4"/>
@@ -1784,7 +1779,7 @@
       <c r="O75" s="9"/>
       <c r="P75" s="9"/>
     </row>
-    <row r="76" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A76" s="4"/>
       <c r="C76" s="4"/>
       <c r="E76" s="4"/>
@@ -1794,7 +1789,7 @@
       <c r="O76" s="9"/>
       <c r="P76" s="9"/>
     </row>
-    <row r="77" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A77" s="4"/>
       <c r="C77" s="4"/>
       <c r="E77" s="4"/>
@@ -1802,7 +1797,7 @@
       <c r="K77" s="6"/>
       <c r="N77" s="7"/>
     </row>
-    <row r="78" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A78" s="4"/>
       <c r="C78" s="4"/>
       <c r="E78" s="4"/>
@@ -1810,7 +1805,7 @@
       <c r="K78" s="6"/>
       <c r="N78" s="7"/>
     </row>
-    <row r="79" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A79" s="4"/>
       <c r="C79" s="4"/>
       <c r="E79" s="4"/>
@@ -1820,7 +1815,7 @@
       <c r="O79" s="9"/>
       <c r="P79" s="9"/>
     </row>
-    <row r="80" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A80" s="4"/>
       <c r="C80" s="4"/>
       <c r="E80" s="4"/>
@@ -1828,7 +1823,7 @@
       <c r="K80" s="6"/>
       <c r="N80" s="7"/>
     </row>
-    <row r="81" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A81" s="4"/>
       <c r="C81" s="4"/>
       <c r="E81" s="4"/>
@@ -1838,7 +1833,7 @@
       <c r="O81" s="9"/>
       <c r="P81" s="9"/>
     </row>
-    <row r="82" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A82" s="4"/>
       <c r="C82" s="4"/>
       <c r="E82" s="4"/>
@@ -1848,7 +1843,7 @@
       <c r="O82" s="9"/>
       <c r="P82" s="9"/>
     </row>
-    <row r="83" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A83" s="4"/>
       <c r="C83" s="4"/>
       <c r="E83" s="4"/>
@@ -1857,7 +1852,7 @@
       <c r="N83" s="8"/>
       <c r="O83" s="9"/>
     </row>
-    <row r="84" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A84" s="4"/>
       <c r="C84" s="4"/>
       <c r="E84" s="4"/>
@@ -1865,7 +1860,7 @@
       <c r="K84" s="6"/>
       <c r="N84" s="7"/>
     </row>
-    <row r="85" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A85" s="4"/>
       <c r="C85" s="4"/>
       <c r="E85" s="4"/>
@@ -1873,7 +1868,7 @@
       <c r="K85" s="6"/>
       <c r="N85" s="7"/>
     </row>
-    <row r="86" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A86" s="4"/>
       <c r="C86" s="4"/>
       <c r="E86" s="4"/>
@@ -1882,7 +1877,7 @@
       <c r="N86" s="8"/>
       <c r="O86" s="9"/>
     </row>
-    <row r="87" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A87" s="4"/>
       <c r="C87" s="4"/>
       <c r="E87" s="4"/>
@@ -1890,7 +1885,7 @@
       <c r="K87" s="6"/>
       <c r="N87" s="7"/>
     </row>
-    <row r="88" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A88" s="4"/>
       <c r="C88" s="4"/>
       <c r="E88" s="4"/>
@@ -1900,7 +1895,7 @@
       <c r="O88" s="9"/>
       <c r="P88" s="9"/>
     </row>
-    <row r="89" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A89" s="4"/>
       <c r="C89" s="4"/>
       <c r="E89" s="4"/>
@@ -1910,7 +1905,7 @@
       <c r="O89" s="9"/>
       <c r="P89" s="9"/>
     </row>
-    <row r="90" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="4"/>
       <c r="C90" s="4"/>
       <c r="E90" s="4"/>
@@ -1920,7 +1915,7 @@
       <c r="O90" s="9"/>
       <c r="P90" s="9"/>
     </row>
-    <row r="91" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="4"/>
       <c r="C91" s="4"/>
       <c r="E91" s="4"/>
@@ -1928,7 +1923,7 @@
       <c r="K91" s="6"/>
       <c r="N91" s="7"/>
     </row>
-    <row r="92" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A92" s="4"/>
       <c r="C92" s="4"/>
       <c r="E92" s="4"/>
@@ -1936,7 +1931,7 @@
       <c r="K92" s="6"/>
       <c r="N92" s="7"/>
     </row>
-    <row r="93" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A93" s="4"/>
       <c r="C93" s="4"/>
       <c r="E93" s="4"/>
@@ -1946,7 +1941,7 @@
       <c r="O93" s="9"/>
       <c r="P93" s="9"/>
     </row>
-    <row r="94" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A94" s="4"/>
       <c r="C94" s="4"/>
       <c r="E94" s="4"/>
@@ -1956,7 +1951,7 @@
       <c r="O94" s="9"/>
       <c r="P94" s="9"/>
     </row>
-    <row r="95" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="4"/>
       <c r="C95" s="4"/>
       <c r="E95" s="4"/>
@@ -1966,7 +1961,7 @@
       <c r="O95" s="9"/>
       <c r="P95" s="9"/>
     </row>
-    <row r="96" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="4"/>
       <c r="C96" s="4"/>
       <c r="E96" s="4"/>
@@ -1976,7 +1971,7 @@
       <c r="O96" s="9"/>
       <c r="P96" s="9"/>
     </row>
-    <row r="97" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="4"/>
       <c r="C97" s="4"/>
       <c r="E97" s="4"/>
@@ -1984,7 +1979,7 @@
       <c r="K97" s="6"/>
       <c r="N97" s="7"/>
     </row>
-    <row r="98" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="4"/>
       <c r="C98" s="4"/>
       <c r="E98" s="4"/>
@@ -1994,7 +1989,7 @@
       <c r="O98" s="9"/>
       <c r="P98" s="9"/>
     </row>
-    <row r="99" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A99" s="4"/>
       <c r="C99" s="4"/>
       <c r="E99" s="4"/>
@@ -2004,7 +1999,7 @@
       <c r="O99" s="9"/>
       <c r="P99" s="9"/>
     </row>
-    <row r="100" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="4"/>
       <c r="C100" s="4"/>
       <c r="E100" s="4"/>
@@ -2012,7 +2007,7 @@
       <c r="K100" s="6"/>
       <c r="N100" s="7"/>
     </row>
-    <row r="101" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A101" s="4"/>
       <c r="C101" s="4"/>
       <c r="E101" s="4"/>
@@ -2021,7 +2016,7 @@
       <c r="N101" s="8"/>
       <c r="O101" s="9"/>
     </row>
-    <row r="102" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A102" s="4"/>
       <c r="C102" s="4"/>
       <c r="E102" s="4"/>
@@ -2031,7 +2026,7 @@
       <c r="O102" s="9"/>
       <c r="P102" s="9"/>
     </row>
-    <row r="103" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A103" s="4"/>
       <c r="C103" s="4"/>
       <c r="E103" s="4"/>
@@ -2040,7 +2035,7 @@
       <c r="N103" s="8"/>
       <c r="O103" s="9"/>
     </row>
-    <row r="104" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A104" s="4"/>
       <c r="C104" s="4"/>
       <c r="E104" s="4"/>
@@ -2048,7 +2043,7 @@
       <c r="K104" s="6"/>
       <c r="N104" s="7"/>
     </row>
-    <row r="105" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A105" s="4"/>
       <c r="C105" s="4"/>
       <c r="E105" s="4"/>
@@ -2058,7 +2053,7 @@
       <c r="O105" s="9"/>
       <c r="P105" s="9"/>
     </row>
-    <row r="106" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A106" s="4"/>
       <c r="C106" s="4"/>
       <c r="E106" s="4"/>
@@ -2068,7 +2063,7 @@
       <c r="O106" s="9"/>
       <c r="P106" s="9"/>
     </row>
-    <row r="107" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A107" s="4"/>
       <c r="C107" s="4"/>
       <c r="E107" s="4"/>
@@ -2076,7 +2071,7 @@
       <c r="K107" s="6"/>
       <c r="N107" s="7"/>
     </row>
-    <row r="108" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A108" s="4"/>
       <c r="C108" s="4"/>
       <c r="E108" s="4"/>
@@ -2086,7 +2081,7 @@
       <c r="O108" s="9"/>
       <c r="P108" s="9"/>
     </row>
-    <row r="109" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A109" s="4"/>
       <c r="C109" s="4"/>
       <c r="E109" s="4"/>
@@ -2094,7 +2089,7 @@
       <c r="K109" s="6"/>
       <c r="N109" s="7"/>
     </row>
-    <row r="110" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A110" s="4"/>
       <c r="C110" s="4"/>
       <c r="E110" s="4"/>
@@ -2104,7 +2099,7 @@
       <c r="O110" s="9"/>
       <c r="P110" s="9"/>
     </row>
-    <row r="111" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A111" s="4"/>
       <c r="C111" s="4"/>
       <c r="E111" s="4"/>
@@ -2114,7 +2109,7 @@
       <c r="O111" s="9"/>
       <c r="P111" s="9"/>
     </row>
-    <row r="112" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A112" s="4"/>
       <c r="C112" s="4"/>
       <c r="E112" s="4"/>
@@ -2122,7 +2117,7 @@
       <c r="K112" s="6"/>
       <c r="N112" s="7"/>
     </row>
-    <row r="113" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A113" s="4"/>
       <c r="C113" s="4"/>
       <c r="E113" s="4"/>
@@ -2130,7 +2125,7 @@
       <c r="K113" s="6"/>
       <c r="N113" s="7"/>
     </row>
-    <row r="114" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A114" s="4"/>
       <c r="C114" s="4"/>
       <c r="E114" s="4"/>
@@ -2138,7 +2133,7 @@
       <c r="K114" s="6"/>
       <c r="N114" s="7"/>
     </row>
-    <row r="115" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A115" s="4"/>
       <c r="C115" s="4"/>
       <c r="E115" s="4"/>
@@ -2148,7 +2143,7 @@
       <c r="O115" s="9"/>
       <c r="P115" s="9"/>
     </row>
-    <row r="116" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A116" s="4"/>
       <c r="C116" s="4"/>
       <c r="E116" s="15"/>
@@ -2158,7 +2153,7 @@
       <c r="O116" s="9"/>
       <c r="P116" s="9"/>
     </row>
-    <row r="117" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A117" s="4"/>
       <c r="C117" s="4"/>
       <c r="E117" s="4"/>
@@ -2167,7 +2162,7 @@
       <c r="N117" s="7"/>
     </row>
   </sheetData>
-  <sortState ref="A2:P125">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:P125">
     <sortCondition ref="C2:C125"/>
     <sortCondition ref="D2:D125"/>
   </sortState>

</xml_diff>